<commit_message>
Added code for data Handlers using excel
</commit_message>
<xml_diff>
--- a/TestData/data.xlsx
+++ b/TestData/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IDE2020 projects\com.SeleniumFrameworkTDDV1.0\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE93BAE-2B41-44CB-A211-399E136BDBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB7123C-615A-4538-B399-F24998F80272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testData" sheetId="1" r:id="rId1"/>
+    <sheet name="writeData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,12 +25,64 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t>rahul</t>
+  </si>
+  <si>
+    <t>ritesh</t>
+  </si>
+  <si>
+    <t>tester</t>
+  </si>
+  <si>
+    <t>rahulriteshqa@gmail.com</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>username1</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>analyst</t>
+  </si>
+  <si>
+    <t>username2</t>
+  </si>
+  <si>
+    <t>password2</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -52,13 +105,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -337,10 +393,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>123</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>125</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>126</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" xr:uid="{652A1038-CA9D-407D-9E65-9AE5BADD7C93}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C2297E-ED28-4EF1-8B2A-FE3C427CE92C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>